<commit_message>
Add PE within crop types
</commit_message>
<xml_diff>
--- a/results/eoe_summaries/addition_eoe_summaries.xlsx
+++ b/results/eoe_summaries/addition_eoe_summaries.xlsx
@@ -8,20 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\pvillanueva13\repos\lamps_incubation\results\eoe_summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{934B1B4E-B6DC-4D91-A805-15FFDF3B2864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E11683B-C85A-47F7-BA19-6195E393D74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{D5005DE2-E3CD-41D0-BAB7-D43F304862F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{D5005DE2-E3CD-41D0-BAB7-D43F304862F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Everything" sheetId="1" r:id="rId1"/>
     <sheet name="Treatment" sheetId="3" r:id="rId2"/>
     <sheet name="Crop" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Crop!$A$1:$D$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Treatment!$A$1:$D$181</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="20" r:id="rId5"/>
+    <pivotCache cacheId="19" r:id="rId6"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="45">
   <si>
     <t>factor</t>
   </si>
@@ -166,11 +171,26 @@
   <si>
     <t>Nitrogen 336N</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of value</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,13 +220,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -217,6 +250,2546 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Paul" refreshedDate="45086.010130439812" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="180" xr:uid="{51134D27-A466-48A0-8521-E787DDB1F218}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="factor" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="level" numFmtId="0">
+      <sharedItems count="9">
+        <s v="Carbon 0N"/>
+        <s v="Carbon 112N"/>
+        <s v="Carbon 336N"/>
+        <s v="Control 0N"/>
+        <s v="Control 112N"/>
+        <s v="Control 336N"/>
+        <s v="Nitrogen 0N"/>
+        <s v="Nitrogen 112N"/>
+        <s v="Nitrogen 336N"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="name" numFmtId="0">
+      <sharedItems count="20">
+        <s v="CO2_flux_ug_g_d_mean"/>
+        <s v="CO2_flux_ug_g_d_sd"/>
+        <s v="cum_CO2_flux_ug_g_mean"/>
+        <s v="cum_CO2_flux_ug_g_sd"/>
+        <s v="N2ON_flux_ug_g_d_mean"/>
+        <s v="N2ON_flux_ug_g_d_sd"/>
+        <s v="cum_N2O_flux_ug_g_mean"/>
+        <s v="cum_N2O_flux_ug_g_sd"/>
+        <s v="net_min_rate_rel_mean"/>
+        <s v="net_min_rate_rel_sd"/>
+        <s v="net_min_rate_abs_mean"/>
+        <s v="net_min_rate_abs_sd"/>
+        <s v="net_nitr_rate_rel_mean"/>
+        <s v="net_nitr_rate_rel_sd"/>
+        <s v="net_nitr_rate_abs_mean"/>
+        <s v="net_nitr_rate_abs_sd"/>
+        <s v="no3n_mg_kg_1_mean"/>
+        <s v="no3n_mg_kg_1_sd"/>
+        <s v="nh4n_mg_kg_1_mean"/>
+        <s v="nh4n_mg_kg_1_sd"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="value" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1.1175604770974801" maxValue="3151.77431838555" count="180">
+        <n v="15.1510687474363"/>
+        <n v="7.0629362264116899"/>
+        <n v="3151.77431838555"/>
+        <n v="1172.95614345217"/>
+        <n v="13.813488988945901"/>
+        <n v="4.46210667823033"/>
+        <n v="2750.5537824144599"/>
+        <n v="1015.97355311231"/>
+        <n v="14.4390506266177"/>
+        <n v="6.2474566983605699"/>
+        <n v="2671.4837495660599"/>
+        <n v="1161.58142904801"/>
+        <n v="14.0847143613386"/>
+        <n v="6.4948379231497704"/>
+        <n v="2847.7978282274298"/>
+        <n v="1035.2197077972501"/>
+        <n v="12.8433723612489"/>
+        <n v="4.9321111188240501"/>
+        <n v="2480.8353651971802"/>
+        <n v="966.454760994656"/>
+        <n v="12.685417710965099"/>
+        <n v="6.3399045571011197"/>
+        <n v="2438.1683539158798"/>
+        <n v="1326.86688047759"/>
+        <n v="14.1934839192862"/>
+        <n v="6.2387897581410101"/>
+        <n v="2848.6559073283101"/>
+        <n v="1128.4327225584"/>
+        <n v="11.626800226485299"/>
+        <n v="5.6151166044812504"/>
+        <n v="2156.4045505998301"/>
+        <n v="1044.3343308766"/>
+        <n v="12.265221449423899"/>
+        <n v="6.35180045064795"/>
+        <n v="2258.0482793381202"/>
+        <n v="1220.34255851953"/>
+        <n v="6.2560285E-3"/>
+        <n v="1.92200444700244E-2"/>
+        <n v="5.9756772499999899E-3"/>
+        <n v="3.2775468944656199"/>
+        <n v="8.8660837499999999E-3"/>
+        <n v="3.3292850263116597E-2"/>
+        <n v="1.4899711848749999"/>
+        <n v="3.4027659475364902"/>
+        <n v="4.3572927499999997E-2"/>
+        <n v="0.10114481318167801"/>
+        <n v="11.092913531500001"/>
+        <n v="23.4122927402335"/>
+        <n v="8.5451950000000002E-3"/>
+        <n v="2.1473061992008699E-2"/>
+        <n v="1.054421853125"/>
+        <n v="2.5575904123563502"/>
+        <n v="1.9778582999999999E-2"/>
+        <n v="4.9286949619634902E-2"/>
+        <n v="5.3442339456249996"/>
+        <n v="9.3827701605982305"/>
+        <n v="0.11387184525000001"/>
+        <n v="0.166410097949592"/>
+        <n v="16.656926738875001"/>
+        <n v="23.6521402322272"/>
+        <n v="5.4609991250000002E-3"/>
+        <n v="1.08292293543856E-2"/>
+        <n v="2.9922594381250001"/>
+        <n v="4.6503342133930801"/>
+        <n v="7.0442747500000001E-3"/>
+        <n v="2.57291353332583E-2"/>
+        <n v="7.5258717323750002"/>
+        <n v="16.7941786546555"/>
+        <n v="8.2240151999999997E-2"/>
+        <n v="0.132767678228495"/>
+        <n v="12.427385524749999"/>
+        <n v="24.807900055071201"/>
+        <n v="0.16183905947535299"/>
+        <n v="1.45458207618155"/>
+        <n v="4.7232424147421996"/>
+        <n v="2.04678587093274"/>
+        <n v="0.156024714068797"/>
+        <n v="1.4335887256153099"/>
+        <n v="4.8173248678982903"/>
+        <n v="2.1181507087288201"/>
+        <n v="153.75220759385999"/>
+        <n v="66.264109766289906"/>
+        <n v="3.6044652426655999"/>
+        <n v="2.8928707781548"/>
+        <n v="-6.7191452282821104E-3"/>
+        <n v="1.37225837627701"/>
+        <n v="4.2363694338207996"/>
+        <n v="3.3700897888071202"/>
+        <n v="-7.7553094220089401E-3"/>
+        <n v="1.3992383543109199"/>
+        <n v="4.3252605898729604"/>
+        <n v="3.4257252772621398"/>
+        <n v="167.01251644459001"/>
+        <n v="105.38120125785601"/>
+        <n v="3.4014390783492998"/>
+        <n v="1.63122000228043"/>
+        <n v="-1.02762622183173"/>
+        <n v="1.60390647947168"/>
+        <n v="4.0574484277109297"/>
+        <n v="3.2710406806154499"/>
+        <n v="-1.1175604770974801"/>
+        <n v="1.65306380469438"/>
+        <n v="4.1969842922220897"/>
+        <n v="3.3383880096329599"/>
+        <n v="175.99567259036201"/>
+        <n v="102.87042708258301"/>
+        <n v="3.46415678458487"/>
+        <n v="2.71809076953588"/>
+        <n v="0.15162544511626"/>
+        <n v="1.3818542606794"/>
+        <n v="5.3522773905481502"/>
+        <n v="2.5011703071260198"/>
+        <n v="0.126926359954183"/>
+        <n v="1.41856330439987"/>
+        <n v="5.4718271314504303"/>
+        <n v="2.5775635570242801"/>
+        <n v="174.93413383433099"/>
+        <n v="81.297569975785095"/>
+        <n v="3.25593702192293"/>
+        <n v="2.9465185710554702"/>
+        <n v="-0.32234081901003497"/>
+        <n v="1.1965951292194501"/>
+        <n v="4.7915555193257102"/>
+        <n v="3.4704253452752001"/>
+        <n v="-0.30558612763072501"/>
+        <n v="1.2249144007430299"/>
+        <n v="4.8716910775088698"/>
+        <n v="3.5220647466472399"/>
+        <n v="175.678459032679"/>
+        <n v="111.23624884895899"/>
+        <n v="3.0588076973170502"/>
+        <n v="1.79876050111265"/>
+        <n v="-0.59833281825070395"/>
+        <n v="1.59596409985697"/>
+        <n v="4.7344735134319604"/>
+        <n v="2.9143787970077901"/>
+        <n v="-0.76348943470103903"/>
+        <n v="1.6406264326250399"/>
+        <n v="4.8060574596977901"/>
+        <n v="2.8768215266647799"/>
+        <n v="197.60013103951599"/>
+        <n v="83.995173446945998"/>
+        <n v="6.8650111141310397"/>
+        <n v="7.9051266393467197"/>
+        <n v="2.3571122673731502"/>
+        <n v="4.83521621870399"/>
+        <n v="7.29317760572998"/>
+        <n v="5.0385586766930297"/>
+        <n v="2.3594050094819998"/>
+        <n v="4.85505096931014"/>
+        <n v="7.4781995602525697"/>
+        <n v="5.09429276988753"/>
+        <n v="251.15161172506799"/>
+        <n v="159.39883875410001"/>
+        <n v="3.05518569807532"/>
+        <n v="1.88061695974864"/>
+        <n v="-0.53303400762754904"/>
+        <n v="2.0849281940500002"/>
+        <n v="5.2881217422225602"/>
+        <n v="3.4135985566168299"/>
+        <n v="-0.59758373135807497"/>
+        <n v="2.0963795141271699"/>
+        <n v="5.4114192482454797"/>
+        <n v="3.3848640466794002"/>
+        <n v="213.157667060172"/>
+        <n v="101.752675542522"/>
+        <n v="3.6374477175341098"/>
+        <n v="3.2113948871432401"/>
+        <n v="-0.52787621661294604"/>
+        <n v="1.79224075443818"/>
+        <n v="4.8139240359496096"/>
+        <n v="2.4971402912505698"/>
+        <n v="-0.60165899419093405"/>
+        <n v="1.82390377079124"/>
+        <n v="5.0181676847635002"/>
+        <n v="2.3556499801551301"/>
+        <n v="232.12627978862099"/>
+        <n v="71.800523322440796"/>
+        <n v="3.4509854800050501"/>
+        <n v="2.5944093355581002"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Paul" refreshedDate="45086.010789814813" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="120" xr:uid="{36E447D5-4DD4-4FFF-AAAC-966343DB2ADA}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table2"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="factor" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="level" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Carbon Corn"/>
+        <s v="Carbon Miscanthus"/>
+        <s v="Control Corn"/>
+        <s v="Control Miscanthus"/>
+        <s v="Nitrogen Corn"/>
+        <s v="Nitrogen Miscanthus"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="name" numFmtId="0">
+      <sharedItems count="20">
+        <s v="CO2_flux_ug_g_d_mean"/>
+        <s v="CO2_flux_ug_g_d_sd"/>
+        <s v="cum_CO2_flux_ug_g_mean"/>
+        <s v="cum_CO2_flux_ug_g_sd"/>
+        <s v="N2ON_flux_ug_g_d_mean"/>
+        <s v="N2ON_flux_ug_g_d_sd"/>
+        <s v="cum_N2O_flux_ug_g_mean"/>
+        <s v="cum_N2O_flux_ug_g_sd"/>
+        <s v="net_min_rate_rel_mean"/>
+        <s v="net_min_rate_rel_sd"/>
+        <s v="net_min_rate_abs_mean"/>
+        <s v="net_min_rate_abs_sd"/>
+        <s v="net_nitr_rate_rel_mean"/>
+        <s v="net_nitr_rate_rel_sd"/>
+        <s v="net_nitr_rate_abs_mean"/>
+        <s v="net_nitr_rate_abs_sd"/>
+        <s v="no3n_mg_kg_1_mean"/>
+        <s v="no3n_mg_kg_1_sd"/>
+        <s v="nh4n_mg_kg_1_mean"/>
+        <s v="nh4n_mg_kg_1_sd"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="value" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.96496818224969805" maxValue="3020.6345410099102"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="180">
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="3"/>
+    <x v="23"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="24"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="25"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="26"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="27"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="28"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="29"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="30"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="31"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="32"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="33"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="34"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="35"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="36"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="37"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="38"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="39"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="40"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="41"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="42"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="43"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="44"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="45"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="46"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="7"/>
+    <x v="47"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="48"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="49"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="6"/>
+    <x v="50"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="7"/>
+    <x v="51"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="52"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="53"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="6"/>
+    <x v="54"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="7"/>
+    <x v="55"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="56"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="57"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="58"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="7"/>
+    <x v="59"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="60"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="61"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="62"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="7"/>
+    <x v="63"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="64"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="65"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="6"/>
+    <x v="66"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="67"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="4"/>
+    <x v="68"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="69"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="6"/>
+    <x v="70"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="7"/>
+    <x v="71"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="72"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="73"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="74"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="75"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="12"/>
+    <x v="76"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="77"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="78"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="15"/>
+    <x v="79"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="16"/>
+    <x v="80"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="17"/>
+    <x v="81"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="18"/>
+    <x v="82"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="0"/>
+    <x v="19"/>
+    <x v="83"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="84"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="85"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="86"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="87"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="88"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="13"/>
+    <x v="89"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="14"/>
+    <x v="90"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="15"/>
+    <x v="91"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="16"/>
+    <x v="92"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="17"/>
+    <x v="93"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="18"/>
+    <x v="94"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="1"/>
+    <x v="19"/>
+    <x v="95"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="8"/>
+    <x v="96"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="97"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="10"/>
+    <x v="98"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="11"/>
+    <x v="99"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="12"/>
+    <x v="100"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="101"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="14"/>
+    <x v="102"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="15"/>
+    <x v="103"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="16"/>
+    <x v="104"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="17"/>
+    <x v="105"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="18"/>
+    <x v="106"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="2"/>
+    <x v="19"/>
+    <x v="107"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="8"/>
+    <x v="108"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="9"/>
+    <x v="109"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="10"/>
+    <x v="110"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="11"/>
+    <x v="111"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="12"/>
+    <x v="112"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="13"/>
+    <x v="113"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="14"/>
+    <x v="114"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="15"/>
+    <x v="115"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="16"/>
+    <x v="116"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="117"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="118"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="3"/>
+    <x v="19"/>
+    <x v="119"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="8"/>
+    <x v="120"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="9"/>
+    <x v="121"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="10"/>
+    <x v="122"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="11"/>
+    <x v="123"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="12"/>
+    <x v="124"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="13"/>
+    <x v="125"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="14"/>
+    <x v="126"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="15"/>
+    <x v="127"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="16"/>
+    <x v="128"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="17"/>
+    <x v="129"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="18"/>
+    <x v="130"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="4"/>
+    <x v="19"/>
+    <x v="131"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="8"/>
+    <x v="132"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="9"/>
+    <x v="133"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="10"/>
+    <x v="134"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="11"/>
+    <x v="135"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="12"/>
+    <x v="136"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="13"/>
+    <x v="137"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="14"/>
+    <x v="138"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="15"/>
+    <x v="139"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="16"/>
+    <x v="140"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="17"/>
+    <x v="141"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="18"/>
+    <x v="142"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="5"/>
+    <x v="19"/>
+    <x v="143"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="8"/>
+    <x v="144"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="9"/>
+    <x v="145"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="10"/>
+    <x v="146"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="11"/>
+    <x v="147"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="12"/>
+    <x v="148"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="13"/>
+    <x v="149"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="14"/>
+    <x v="150"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="15"/>
+    <x v="151"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="16"/>
+    <x v="152"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="17"/>
+    <x v="153"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="18"/>
+    <x v="154"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="6"/>
+    <x v="19"/>
+    <x v="155"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="8"/>
+    <x v="156"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="9"/>
+    <x v="157"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="10"/>
+    <x v="158"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="11"/>
+    <x v="159"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="12"/>
+    <x v="160"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="13"/>
+    <x v="161"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="14"/>
+    <x v="162"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="15"/>
+    <x v="163"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="16"/>
+    <x v="164"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="17"/>
+    <x v="165"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="18"/>
+    <x v="166"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="7"/>
+    <x v="19"/>
+    <x v="167"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="168"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="9"/>
+    <x v="169"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="10"/>
+    <x v="170"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="11"/>
+    <x v="171"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="12"/>
+    <x v="172"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="13"/>
+    <x v="173"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="14"/>
+    <x v="174"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="15"/>
+    <x v="175"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="16"/>
+    <x v="176"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="17"/>
+    <x v="177"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="18"/>
+    <x v="178"/>
+  </r>
+  <r>
+    <s v="Treatment"/>
+    <x v="8"/>
+    <x v="19"/>
+    <x v="179"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="120">
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="13.0519008893069"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="4.7576498247689099"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="2695.24002590081"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="917.73943135929403"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="15.8838380193597"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="6.5494131748963804"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3020.6345410099102"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1259.9494005689901"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="11.5507306145154"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4.4427505059141996"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2332.2588495935302"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="790.94685402502796"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="14.8582723411863"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="6.5613257789898096"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="2845.6088486334602"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1304.2833513426599"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="10.3707031200305"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="4.6404645153052302"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="2157.2864795375199"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="931.27280900375797"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="15.019633943433099"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="6.3073056874866298"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="2684.78601197331"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1279.1598310033901"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="1.0946257583333299E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="2.63744055532939E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="1.0219196216666699"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="7"/>
+    <n v="3.9654620090252402"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="2.8183768916666699E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="8.4995185281643196E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="7.3706539740833303"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="19.442115055854899"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="3.7239970249999997E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="8.1324292005264795E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="4.6854842260833296"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="7"/>
+    <n v="10.502658544891901"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="5.7557111916666702E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="0.132246570959871"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="10.684904132333299"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="19.512702182096199"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="1.7886153916666699E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="5"/>
+    <n v="3.7842821941658299E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="6"/>
+    <n v="2.80739561075"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="7"/>
+    <n v="3.68445526453656"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="4.5277463333333302E-2"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="0.112571708528391"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="6"/>
+    <n v="12.4896155194167"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="7"/>
+    <n v="23.5066352835813"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="8"/>
+    <n v="-0.93234169433182801"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="9"/>
+    <n v="0.77925870048246404"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="10"/>
+    <n v="4.9480117632619596"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="11"/>
+    <n v="1.97567371354608"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="12"/>
+    <n v="-0.96496818224969805"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="13"/>
+    <n v="0.81691629502682495"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="14"/>
+    <n v="5.01163636257108"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="15"/>
+    <n v="1.9474210544961199"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="16"/>
+    <n v="176.41665790265199"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="17"/>
+    <n v="58.702198861132203"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="18"/>
+    <n v="3.7611134696730399"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="0"/>
+    <x v="19"/>
+    <n v="1.4522655290216699"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="0.35067082260871901"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="9"/>
+    <n v="1.8108634254431299"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="10"/>
+    <n v="3.73002842092066"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="11"/>
+    <n v="3.48748844360273"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="12"/>
+    <n v="0.31877413394923698"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="13"/>
+    <n v="1.85060611673727"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="14"/>
+    <n v="3.88141013742448"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="15"/>
+    <n v="3.6169207799762799"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="16"/>
+    <n v="154.75693984988899"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="17"/>
+    <n v="114.348896380078"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="18"/>
+    <n v="3.2189272673934699"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="1"/>
+    <x v="19"/>
+    <n v="3.0767820520744902"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="8"/>
+    <n v="-0.86452746509015999"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="9"/>
+    <n v="0.83328937685808602"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="10"/>
+    <n v="5.6136087927450804"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="11"/>
+    <n v="2.3366988100991"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="12"/>
+    <n v="-0.94737463625406904"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="13"/>
+    <n v="0.85148280759327699"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="14"/>
+    <n v="5.6431140578458603"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="15"/>
+    <n v="2.3091540056390101"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="16"/>
+    <n v="195.127483428853"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="17"/>
+    <n v="70.472131447489602"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="18"/>
+    <n v="5.4950043884911901"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="2"/>
+    <x v="19"/>
+    <n v="6.32889913110274"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="8"/>
+    <n v="0.35182867032717402"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="9"/>
+    <n v="1.5668738138236999"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="10"/>
+    <n v="4.3052621561254698"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="11"/>
+    <n v="3.29028448353364"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="12"/>
+    <n v="0.31927516800234801"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="13"/>
+    <n v="1.6237247666912"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="14"/>
+    <n v="4.4566030545922004"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="15"/>
+    <n v="3.3888465279373299"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="16"/>
+    <n v="170.34766584216499"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="17"/>
+    <n v="107.282592940608"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="18"/>
+    <n v="3.2914995004228298"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="3"/>
+    <x v="19"/>
+    <n v="3.3655084583620201"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="8"/>
+    <n v="-0.333607669611102"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="9"/>
+    <n v="2.75531517917715"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="10"/>
+    <n v="5.9797293653829096"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="11"/>
+    <n v="2.0798172604456302"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="12"/>
+    <n v="-0.39346062920755498"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="13"/>
+    <n v="2.8029210498884298"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="14"/>
+    <n v="6.0790058157981903"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="15"/>
+    <n v="1.96674802307979"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="16"/>
+    <n v="223.91633217375701"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="17"/>
+    <n v="46.8768525482878"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="18"/>
+    <n v="4.3236011875111497"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="4"/>
+    <x v="19"/>
+    <n v="2.7700438334476898"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="8"/>
+    <n v="1.19774236503287"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="9"/>
+    <n v="3.85485153227128"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="10"/>
+    <n v="5.61708622388519"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="11"/>
+    <n v="5.0656460125719196"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="12"/>
+    <n v="1.1669021518295499"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="13"/>
+    <n v="3.86969701884103"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="14"/>
+    <n v="5.8595185130428398"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="15"/>
+    <n v="5.0973312100947501"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="16"/>
+    <n v="240.37404020881601"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="17"/>
+    <n v="155.62062781521001"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="18"/>
+    <n v="2.4388114095651701"/>
+  </r>
+  <r>
+    <s v="Crop"/>
+    <x v="5"/>
+    <x v="19"/>
+    <n v="1.9012086842021201"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BF85F007-3A7B-43EA-9DDF-20F29EFE3A51}" name="PivotTable5" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A17:D25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="21">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="3"/>
+        <item x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="14"/>
+        <item h="1" x="15"/>
+        <item h="1" x="12"/>
+        <item h="1" x="13"/>
+        <item h="1" x="18"/>
+        <item h="1" x="19"/>
+        <item h="1" x="16"/>
+        <item h="1" x="17"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of value" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF7FD731-85C2-4F92-8FC4-61BF76B4797D}" name="PivotTable4" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="21">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="3"/>
+        <item x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="14"/>
+        <item h="1" x="15"/>
+        <item h="1" x="12"/>
+        <item h="1" x="13"/>
+        <item h="1" x="18"/>
+        <item h="1" x="19"/>
+        <item h="1" x="16"/>
+        <item h="1" x="17"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="181">
+        <item x="100"/>
+        <item x="96"/>
+        <item x="136"/>
+        <item x="172"/>
+        <item x="132"/>
+        <item x="160"/>
+        <item x="156"/>
+        <item x="168"/>
+        <item x="120"/>
+        <item x="124"/>
+        <item x="88"/>
+        <item x="84"/>
+        <item x="60"/>
+        <item x="38"/>
+        <item x="36"/>
+        <item x="64"/>
+        <item x="48"/>
+        <item x="40"/>
+        <item x="61"/>
+        <item x="37"/>
+        <item x="52"/>
+        <item x="49"/>
+        <item x="65"/>
+        <item x="41"/>
+        <item x="44"/>
+        <item x="53"/>
+        <item x="68"/>
+        <item x="45"/>
+        <item x="56"/>
+        <item x="112"/>
+        <item x="69"/>
+        <item x="108"/>
+        <item x="76"/>
+        <item x="72"/>
+        <item x="57"/>
+        <item x="50"/>
+        <item x="121"/>
+        <item x="125"/>
+        <item x="85"/>
+        <item x="109"/>
+        <item x="89"/>
+        <item x="113"/>
+        <item x="77"/>
+        <item x="73"/>
+        <item x="42"/>
+        <item x="133"/>
+        <item x="97"/>
+        <item x="95"/>
+        <item x="137"/>
+        <item x="101"/>
+        <item x="169"/>
+        <item x="131"/>
+        <item x="173"/>
+        <item x="155"/>
+        <item x="75"/>
+        <item x="157"/>
+        <item x="161"/>
+        <item x="79"/>
+        <item x="175"/>
+        <item x="144"/>
+        <item x="148"/>
+        <item x="171"/>
+        <item x="111"/>
+        <item x="51"/>
+        <item x="115"/>
+        <item x="179"/>
+        <item x="107"/>
+        <item x="139"/>
+        <item x="83"/>
+        <item x="135"/>
+        <item x="119"/>
+        <item x="62"/>
+        <item x="154"/>
+        <item x="130"/>
+        <item x="167"/>
+        <item x="118"/>
+        <item x="99"/>
+        <item x="39"/>
+        <item x="103"/>
+        <item x="87"/>
+        <item x="163"/>
+        <item x="94"/>
+        <item x="43"/>
+        <item x="159"/>
+        <item x="91"/>
+        <item x="178"/>
+        <item x="106"/>
+        <item x="123"/>
+        <item x="127"/>
+        <item x="82"/>
+        <item x="166"/>
+        <item x="98"/>
+        <item x="102"/>
+        <item x="86"/>
+        <item x="90"/>
+        <item x="5"/>
+        <item x="63"/>
+        <item x="74"/>
+        <item x="134"/>
+        <item x="122"/>
+        <item x="138"/>
+        <item x="170"/>
+        <item x="78"/>
+        <item x="145"/>
+        <item x="149"/>
+        <item x="126"/>
+        <item x="17"/>
+        <item x="174"/>
+        <item x="147"/>
+        <item x="151"/>
+        <item x="158"/>
+        <item x="54"/>
+        <item x="110"/>
+        <item x="162"/>
+        <item x="114"/>
+        <item x="29"/>
+        <item x="25"/>
+        <item x="9"/>
+        <item x="21"/>
+        <item x="33"/>
+        <item x="13"/>
+        <item x="142"/>
+        <item x="1"/>
+        <item x="146"/>
+        <item x="150"/>
+        <item x="66"/>
+        <item x="143"/>
+        <item x="55"/>
+        <item x="46"/>
+        <item x="28"/>
+        <item x="32"/>
+        <item x="70"/>
+        <item x="20"/>
+        <item x="16"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="24"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item x="58"/>
+        <item x="67"/>
+        <item x="47"/>
+        <item x="59"/>
+        <item x="71"/>
+        <item x="81"/>
+        <item x="177"/>
+        <item x="117"/>
+        <item x="141"/>
+        <item x="165"/>
+        <item x="105"/>
+        <item x="93"/>
+        <item x="129"/>
+        <item x="80"/>
+        <item x="153"/>
+        <item x="92"/>
+        <item x="116"/>
+        <item x="128"/>
+        <item x="104"/>
+        <item x="140"/>
+        <item x="164"/>
+        <item x="176"/>
+        <item x="152"/>
+        <item x="19"/>
+        <item x="7"/>
+        <item x="15"/>
+        <item x="31"/>
+        <item x="27"/>
+        <item x="11"/>
+        <item x="3"/>
+        <item x="35"/>
+        <item x="23"/>
+        <item x="30"/>
+        <item x="34"/>
+        <item x="22"/>
+        <item x="18"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="26"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of value" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B27EEC1B-5E6A-4079-8C95-FDC5B1661C96}" name="Table1" displayName="Table1" ref="A1:D181" totalsRowShown="0">
+  <autoFilter ref="A1:D181" xr:uid="{C539C25E-8D5E-4B71-8013-8D488243F151}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{41F1415E-467D-4ABF-9343-6DC8D34D8C84}" name="factor"/>
+    <tableColumn id="2" xr3:uid="{5C0A62AB-D2DA-4F81-9B6F-679700F17811}" name="level"/>
+    <tableColumn id="3" xr3:uid="{7E098EB7-C01A-4DEE-9B23-C78E4162ED81}" name="name"/>
+    <tableColumn id="4" xr3:uid="{971029F3-9F76-4FAF-A003-85B540D06354}" name="value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F05A47EB-81B5-4E04-9C56-F16E3D37D73D}" name="Table2" displayName="Table2" ref="A1:D121" totalsRowShown="0">
+  <autoFilter ref="A1:D121" xr:uid="{E43CF25B-63A6-43FF-B411-4F202440B6DE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{1480D00B-C8FE-4CD0-B3FF-B18B41DC5422}" name="factor"/>
+    <tableColumn id="2" xr3:uid="{5BC72FD3-4C6E-4B9A-9C69-EB53C9295622}" name="level"/>
+    <tableColumn id="3" xr3:uid="{4AFD9C1D-EB9E-4353-91DC-72D6D14D4791}" name="name"/>
+    <tableColumn id="4" xr3:uid="{01FEA0C7-5A87-48CC-BFA2-19CC420BE8A1}" name="value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4747,11 +7320,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C539C25E-8D5E-4B71-8013-8D488243F151}">
   <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C14" sqref="A2:D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7288,8 +9867,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D181" xr:uid="{C539C25E-8D5E-4B71-8013-8D488243F151}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -7297,11 +9878,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43CF25B-63A6-43FF-B411-4F202440B6DE}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -8998,7 +11585,330 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D121" xr:uid="{E43CF25B-63A6-43FF-B411-4F202440B6DE}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9820478F-6E0D-46E1-9666-1D2A31B19546}">
+  <dimension ref="A3:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3151.77431838555</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5.9756772499999899E-3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3151.7802940627998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2750.5537824144599</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.4899711848749999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2752.0437535993347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2671.4837495660599</v>
+      </c>
+      <c r="C7" s="4">
+        <v>11.092913531500001</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2682.57666309756</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2847.7978282274298</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.054421853125</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2848.8522500805548</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2480.8353651971802</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5.3442339456249996</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2486.1795991428053</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2438.1683539158798</v>
+      </c>
+      <c r="C10" s="4">
+        <v>16.656926738875001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2454.8252806547548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2848.6559073283101</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.9922594381250001</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2851.6481667664352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2156.4045505998301</v>
+      </c>
+      <c r="C12" s="4">
+        <v>7.5258717323750002</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2163.9304223322051</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2258.0482793381202</v>
+      </c>
+      <c r="C13" s="4">
+        <v>12.427385524749999</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2270.4756648628704</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3">
+        <v>23603.722134972821</v>
+      </c>
+      <c r="C14" s="3">
+        <v>58.589959626500004</v>
+      </c>
+      <c r="D14" s="3">
+        <v>23662.312094599318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4">
+        <v>2695.24002590081</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1.0219196216666699</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2696.2619455224767</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4">
+        <v>3020.6345410099102</v>
+      </c>
+      <c r="C20" s="4">
+        <v>7.3706539740833303</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3028.0051949839935</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2332.2588495935302</v>
+      </c>
+      <c r="C21" s="4">
+        <v>4.6854842260833296</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2336.9443338196133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2845.6088486334602</v>
+      </c>
+      <c r="C22" s="4">
+        <v>10.684904132333299</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2856.2937527657937</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2157.2864795375199</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2.80739561075</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2160.0938751482699</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2684.78601197331</v>
+      </c>
+      <c r="C24" s="4">
+        <v>12.4896155194167</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2697.2756274927265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="3">
+        <v>15735.81475664854</v>
+      </c>
+      <c r="C25" s="3">
+        <v>39.059973084333329</v>
+      </c>
+      <c r="D25" s="3">
+        <v>15774.874729732874</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>